<commit_message>
Updated Enter Expense Account WorkFlow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testb\Documents\UiPath\FederalBotFactory\AssetsCreation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D053514-BD73-4374-A5B0-8B902476E338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7548B9-338A-4464-B327-BB667162B988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1736,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z16413"/>
   <sheetViews>
-    <sheetView topLeftCell="A271" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B283" sqref="B283"/>
+    <sheetView tabSelected="1" topLeftCell="A210" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D204" sqref="D204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3246,7 +3246,7 @@
         <v>250</v>
       </c>
       <c r="B195">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C195" t="s">
         <v>71</v>
@@ -3257,7 +3257,7 @@
         <v>253</v>
       </c>
       <c r="B196">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C196" t="s">
         <v>71</v>
@@ -3268,7 +3268,7 @@
         <v>254</v>
       </c>
       <c r="B197">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C197" t="s">
         <v>71</v>
@@ -3279,7 +3279,7 @@
         <v>255</v>
       </c>
       <c r="B198">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C198" t="s">
         <v>71</v>
@@ -3290,7 +3290,7 @@
         <v>256</v>
       </c>
       <c r="B199">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C199" t="s">
         <v>71</v>
@@ -3301,7 +3301,7 @@
         <v>257</v>
       </c>
       <c r="B200">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C200" t="s">
         <v>71</v>
@@ -3312,7 +3312,7 @@
         <v>258</v>
       </c>
       <c r="B201">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C201" t="s">
         <v>71</v>
@@ -3323,7 +3323,7 @@
         <v>234</v>
       </c>
       <c r="B202">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C202" t="s">
         <v>71</v>
@@ -3334,7 +3334,7 @@
         <v>241</v>
       </c>
       <c r="B203">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C203" t="s">
         <v>47</v>
@@ -3345,7 +3345,7 @@
         <v>161</v>
       </c>
       <c r="B204">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C204" t="s">
         <v>47</v>
@@ -3356,7 +3356,7 @@
         <v>173</v>
       </c>
       <c r="B205">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C205" t="s">
         <v>71</v>
@@ -3367,7 +3367,7 @@
         <v>172</v>
       </c>
       <c r="B206">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C206" t="s">
         <v>71</v>
@@ -3378,7 +3378,7 @@
         <v>176</v>
       </c>
       <c r="B207">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C207" t="s">
         <v>71</v>
@@ -3389,7 +3389,7 @@
         <v>179</v>
       </c>
       <c r="B208">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C208" t="s">
         <v>71</v>
@@ -3400,7 +3400,7 @@
         <v>182</v>
       </c>
       <c r="B209">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C209" t="s">
         <v>71</v>
@@ -3411,7 +3411,7 @@
         <v>185</v>
       </c>
       <c r="B210">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C210" t="s">
         <v>71</v>
@@ -3422,7 +3422,7 @@
         <v>188</v>
       </c>
       <c r="B211">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C211" t="s">
         <v>71</v>
@@ -3433,7 +3433,7 @@
         <v>191</v>
       </c>
       <c r="B212">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C212" t="s">
         <v>71</v>
@@ -3444,7 +3444,7 @@
         <v>194</v>
       </c>
       <c r="B213">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C213" t="s">
         <v>71</v>
@@ -54560,7 +54560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B5CA207-C514-463D-8AD4-AD89DA25ADFE}">
   <dimension ref="A1:A47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>